<commit_message>
* Add logs, fixing issue on test repeats * Fixing issues on GUI test, change GUI confidence level to 0.95 * Allow setting resources path for drivers, to be downloaded separately * Added support to Firefox, Safari, (IE, firefox, edge to be tested in Windows)
</commit_message>
<xml_diff>
--- a/PyAutoTest/tests/AutoTestTemplate.xlsx
+++ b/PyAutoTest/tests/AutoTestTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samantha/Dev/PycharmProjects/PyAutoTest2020/PyAutoTest/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814EA45E-A0FE-D74D-8D13-A46B1371DEE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A3BD38-6191-6448-93A1-72C018844F3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="118">
   <si>
     <t>RepeatDataSheetName</t>
   </si>
@@ -164,18 +164,12 @@
     <t>Options:</t>
   </si>
   <si>
-    <t>Others</t>
-  </si>
-  <si>
     <t>Repeat Data sheet name Referenced in "Case"</t>
   </si>
   <si>
     <t>1) Run</t>
   </si>
   <si>
-    <t>(Empty)</t>
-  </si>
-  <si>
     <t>2) RunInit</t>
   </si>
   <si>
@@ -200,9 +194,6 @@
     <t>(Please make sure no duplicates)</t>
   </si>
   <si>
-    <t>6)</t>
-  </si>
-  <si>
     <t>7) Case</t>
   </si>
   <si>
@@ -344,9 +335,6 @@
     <t>http://www.yahoo.com.hk</t>
   </si>
   <si>
-    <t>web, winm gui</t>
-  </si>
-  <si>
     <t>Click mail</t>
   </si>
   <si>
@@ -357,13 +345,52 @@
   </si>
   <si>
     <t>wait</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>Clck settings</t>
+  </si>
+  <si>
+    <t>setting.png</t>
+  </si>
+  <si>
+    <t>** must enter something, reading will stop if first column is empty</t>
+  </si>
+  <si>
+    <t>6) RepeatDataSheetName</t>
+  </si>
+  <si>
+    <t>(sheet tab name)</t>
+  </si>
+  <si>
+    <t>(Others)</t>
+  </si>
+  <si>
+    <t>web, win, gui</t>
+  </si>
+  <si>
+    <t>** If Additional Column is added, will include in Result sheet as well</t>
+  </si>
+  <si>
+    <t>Firefox</t>
+  </si>
+  <si>
+    <t>Safari</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>Edge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,13 +414,59 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -409,10 +482,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -694,409 +776,574 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A13:M65"/>
+  <dimension ref="A2:M58"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I68" sqref="I68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
     <col min="3" max="3" width="35.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="12" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C5" s="10"/>
+      <c r="D5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>39</v>
-      </c>
+      <c r="C13" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="C14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="16" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C18" s="10"/>
+      <c r="D18" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
+      <c r="E18" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C21" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C22" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C23" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="25" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>2</v>
-      </c>
-      <c r="B26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C27" s="10"/>
+      <c r="D27" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C31" t="s">
         <v>61</v>
       </c>
-      <c r="D31" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C32" t="s">
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C32" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" s="7"/>
+      <c r="F32" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C33" s="5"/>
+      <c r="D33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C34" s="5"/>
+      <c r="D34" s="6" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>3</v>
-      </c>
-      <c r="B34" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C35" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C37" t="s">
-        <v>43</v>
-      </c>
-      <c r="F37" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C38" t="s">
+      <c r="E34" s="6"/>
+      <c r="F34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C35" s="5"/>
+      <c r="D35" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="6"/>
+      <c r="F35" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C36" s="5"/>
+      <c r="D36" s="6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C40" t="s">
+      <c r="E36" s="6"/>
+      <c r="F36" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C37" s="5"/>
+      <c r="D37" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="6"/>
+      <c r="F37" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C38" s="5"/>
+      <c r="D38" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E38" s="6"/>
+      <c r="F38" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C39" s="5"/>
+      <c r="D39" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" s="6"/>
+      <c r="F39" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C40" s="5"/>
+      <c r="D40" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E40" s="6"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C41" s="5"/>
+      <c r="D41" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E41" s="6"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C42" s="5"/>
+      <c r="D42" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E42" s="6"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C43" s="5"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C45" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" s="7"/>
+      <c r="F45" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C46" s="5"/>
+      <c r="D46" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E46" s="6"/>
+      <c r="F46" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G46" s="3"/>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C47" s="5"/>
+      <c r="D47" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D40" t="s">
-        <v>65</v>
-      </c>
-      <c r="F40" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D41" t="s">
-        <v>15</v>
-      </c>
-      <c r="F41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D42" t="s">
-        <v>66</v>
-      </c>
-      <c r="F42" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D43" t="s">
-        <v>21</v>
-      </c>
-      <c r="F43" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D44" t="s">
-        <v>67</v>
-      </c>
-      <c r="F44" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D45" t="s">
-        <v>38</v>
-      </c>
-      <c r="F45" t="s">
+      <c r="E47" s="6"/>
+      <c r="F47" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D46" t="s">
-        <v>68</v>
-      </c>
-      <c r="F46" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D47" t="s">
-        <v>69</v>
-      </c>
-      <c r="F47" t="s">
+      <c r="G47" s="3"/>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C48" s="5"/>
+      <c r="D48" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E48" s="6"/>
+      <c r="F48" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D48" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D49" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D50" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E51" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C52" t="s">
+      <c r="G48" s="3"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C49" s="5"/>
+      <c r="D49" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D52" t="s">
-        <v>65</v>
-      </c>
-      <c r="F52" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D53" t="s">
+      <c r="E49" s="6"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C50" s="5"/>
+      <c r="D50" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F53" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D54" t="s">
+      <c r="E50" s="6"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C51" s="5"/>
+      <c r="D51" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F54" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D55" t="s">
-        <v>36</v>
-      </c>
-      <c r="F55" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D56" t="s">
+      <c r="E51" s="6"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C52" s="5"/>
+      <c r="D52" s="6" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D57" t="s">
+      <c r="E52" s="6"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C53" s="5"/>
+      <c r="D53" s="6" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D58" t="s">
+      <c r="E53" s="6"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C54" s="5"/>
+      <c r="D54" s="6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D59" t="s">
+      <c r="E54" s="6"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C55" s="5"/>
+      <c r="D55" s="6" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D60" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D61" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D62" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B65" t="s">
+      <c r="E55" s="6"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+    </row>
+    <row r="58" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B58" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" t="s">
         <v>44</v>
-      </c>
-      <c r="C65" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H16" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H6" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
@@ -1113,7 +1360,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1151,42 +1398,48 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2">
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>31</v>
       </c>
-      <c r="F2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G2">
+      <c r="F3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="H2">
+      <c r="H3">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-    </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
       <c r="B4" t="s">
         <v>28</v>
       </c>
@@ -1197,12 +1450,12 @@
         <v>33</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E4" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 E2:E4" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
@@ -1216,10 +1469,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1269,7 +1522,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -1284,7 +1537,21 @@
         <v>6</v>
       </c>
       <c r="G3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4">
         <v>7</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1297,10 +1564,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1331,7 +1598,7 @@
         <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
@@ -1366,7 +1633,7 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J2" t="s">
         <v>11</v>
@@ -1409,19 +1676,19 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" t="s">
         <v>91</v>
-      </c>
-      <c r="F4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" t="s">
-        <v>93</v>
-      </c>
-      <c r="H4" t="s">
-        <v>92</v>
-      </c>
-      <c r="I4" t="s">
-        <v>94</v>
       </c>
       <c r="J4" t="s">
         <v>11</v>
@@ -1447,7 +1714,7 @@
         <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J5" t="s">
         <v>10</v>
@@ -1481,16 +1748,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G7" t="s">
         <v>38</v>
@@ -1504,18 +1771,41 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>102</v>
+      </c>
+      <c r="D8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" t="s">
+        <v>83</v>
       </c>
       <c r="G8" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="J8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="J9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1553,7 +1843,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1579,7 +1869,7 @@
         <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1587,7 +1877,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1595,7 +1885,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>